<commit_message>
Did measurements at 1.2kV
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Ratio</t>
   </si>
@@ -99,6 +99,39 @@
   </si>
   <si>
     <t>300 /4530=0.0662</t>
+  </si>
+  <si>
+    <t>High Voltage (1200V)</t>
+  </si>
+  <si>
+    <t>1120V</t>
+  </si>
+  <si>
+    <t>Expected(1200V)</t>
+  </si>
+  <si>
+    <t>581.5 (changing)</t>
+  </si>
+  <si>
+    <t>836 (changing)</t>
+  </si>
+  <si>
+    <t>740 (changing)</t>
+  </si>
+  <si>
+    <t>640 (changing)</t>
+  </si>
+  <si>
+    <t>508.6 (changing)</t>
+  </si>
+  <si>
+    <t>443.6 (changing)</t>
+  </si>
+  <si>
+    <t>381 (changing)</t>
+  </si>
+  <si>
+    <t>319 (changing)</t>
   </si>
 </sst>
 </file>
@@ -421,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -433,9 +466,10 @@
     <col min="5" max="5" width="27.1640625" customWidth="1"/>
     <col min="6" max="6" width="29.5" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -455,8 +489,14 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -478,8 +518,15 @@
       <c r="G2" s="3">
         <v>8.7989999999999995</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <f>E2*120</f>
+        <v>1055.28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -501,8 +548,15 @@
       <c r="G3" s="3">
         <v>5.3440000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <f t="shared" ref="I3:I10" si="0">E3*120</f>
+        <v>641.28000000000009</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -524,8 +578,15 @@
       <c r="G4" s="3">
         <v>4.4279999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>531.12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -547,8 +608,15 @@
       <c r="G5" s="3">
         <v>3.5579999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>426</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -570,8 +638,15 @@
       <c r="G6" s="3">
         <v>2.9860000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>358.08</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -593,8 +668,15 @@
       <c r="G7" s="3">
         <v>2.4180000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>289.56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -616,8 +698,15 @@
       <c r="G8" s="3">
         <v>1.84</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>220.92</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -639,8 +728,15 @@
       <c r="G9" s="3">
         <v>1.252</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>150.24</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -661,6 +757,13 @@
       </c>
       <c r="G10" s="3">
         <v>0.64529999999999998</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>77.28</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>